<commit_message>
Add Accounts - Customer
New file
</commit_message>
<xml_diff>
--- a/test-cases/Accounts - Customer.xlsx
+++ b/test-cases/Accounts - Customer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Test Cases\admin-system-test-cases\test-cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB14160C-3574-4B4D-8D1D-E25B863B0BFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F97DAC26-AC6E-457A-8D04-52C92EAA321D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{F72C4C41-7DAA-4BA6-B09A-F9391B3B24EA}"/>
   </bookViews>
@@ -563,7 +563,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -706,11 +706,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -773,6 +788,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1088,13 +1106,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{584F85C7-AABF-4034-9BA6-4AAD4E0C232F}">
-  <dimension ref="A1:AC24"/>
+  <dimension ref="A1:AC29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="E18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB25" sqref="AB25"/>
+      <selection pane="bottomRight" activeCell="AB24" sqref="A1:AB24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2260,6 +2278,10 @@
         <v>159</v>
       </c>
     </row>
+    <row r="28" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA29" s="23"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="169" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>